<commit_message>
adding python script to edit .ini file
</commit_message>
<xml_diff>
--- a/benchmark/TableBenchmarkVersions.xlsx
+++ b/benchmark/TableBenchmarkVersions.xlsx
@@ -396,7 +396,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="1" sqref="D1 F6"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -555,7 +555,7 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>

</xml_diff>